<commit_message>
Eval results and Documentation
</commit_message>
<xml_diff>
--- a/Deliverables/Code Review/Evaluation.xlsx
+++ b/Deliverables/Code Review/Evaluation.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Brandon\Desktop\Software Engineering COSC412\Group Project\Project repo\Group-3-Repository\Deliverables\Code Review\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC5378E0-3D71-417B-BE95-C6AFCFDA3D1B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C8777C6E-3A0F-47EF-B91C-7969E1917708}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="2" xr2:uid="{31CC967A-23D1-4812-8F73-68A6D0814E2C}"/>
   </bookViews>
@@ -19,7 +19,7 @@
     <sheet name="Map" sheetId="3" r:id="rId4"/>
     <sheet name="Game" sheetId="1" r:id="rId5"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="191029" iterateDelta="1E-4"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -330,22 +330,22 @@
     <t xml:space="preserve">Keep plugins current and ensure compatability </t>
   </si>
   <si>
-    <t>Primary format provided by Neve plugin</t>
-  </si>
-  <si>
     <t xml:space="preserve">Provide further documentation </t>
   </si>
   <si>
     <t>Keeping Design Consistent</t>
   </si>
   <si>
-    <t>Neve compatability with other plugins</t>
-  </si>
-  <si>
     <t>Prompt to join displayed for all users regardless of membership level</t>
   </si>
   <si>
     <t>Display join now prompt to site visitors only</t>
+  </si>
+  <si>
+    <t>Primary format provided by Template Patterns and Collections plugin</t>
+  </si>
+  <si>
+    <t>Template Patterns and Collections compatability with other plugins</t>
   </si>
 </sst>
 </file>
@@ -1164,7 +1164,7 @@
   <dimension ref="A1:D16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1232,10 +1232,10 @@
         <v>2</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>97</v>
+        <v>101</v>
       </c>
       <c r="C7" s="7" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="30" x14ac:dyDescent="0.25">
@@ -1257,7 +1257,7 @@
         <v>43</v>
       </c>
       <c r="C9" s="7" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="30" x14ac:dyDescent="0.25">
@@ -1309,10 +1309,10 @@
         <v>9</v>
       </c>
       <c r="B14" s="6" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="C14" s="7" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
@@ -1323,7 +1323,7 @@
         <v>89</v>
       </c>
       <c r="C15" s="7" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">

</xml_diff>